<commit_message>
Corrected the estimated and actual hours
</commit_message>
<xml_diff>
--- a/documents/StatusTracker.xlsx
+++ b/documents/StatusTracker.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="92">
   <si>
     <t>PROJECT NUMBER</t>
   </si>
@@ -1380,10 +1380,10 @@
         <v>40</v>
       </c>
       <c r="D55" s="9">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="E55" s="9">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="F55" s="9" t="s">
         <v>47</v>
@@ -1403,17 +1403,15 @@
         <v>19</v>
       </c>
       <c r="D56" s="9">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="E56" s="9">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>82</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G56" s="9"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="9" t="s">
@@ -1426,10 +1424,10 @@
         <v>30</v>
       </c>
       <c r="D57" s="9">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="E57" s="9">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>20</v>
@@ -1477,10 +1475,10 @@
         <v>19</v>
       </c>
       <c r="D60" s="9">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="E60" s="9">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="F60" s="9" t="s">
         <v>20</v>
@@ -1497,10 +1495,10 @@
         <v>30</v>
       </c>
       <c r="D61" s="9">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="E61" s="9">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="F61" s="9" t="s">
         <v>20</v>

</xml_diff>